<commit_message>
Customer Feedback Updated for 10th March Meeting
</commit_message>
<xml_diff>
--- a/Agile Meetings/minutes.xlsx
+++ b/Agile Meetings/minutes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Pictures\Bank-App\Agile Meetings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C073787-85A5-4ED8-B6C7-4E86A2495602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14910778-76D6-42ED-89C0-619478B7F342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="01Mar23" sheetId="2" r:id="rId2"/>
     <sheet name="04Mar23" sheetId="3" r:id="rId3"/>
     <sheet name="10Mar23" sheetId="4" r:id="rId4"/>
+    <sheet name="13Mar23" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -258,10 +259,6 @@
 ii. Commit was made to github repository.</t>
   </si>
   <si>
-    <t>i. Narinder &amp; OZ presented the html design to the customer.
-ii. Customer requested for the 'Register' page to be updated so as to accommodate field for Date of Birth, Type of Account (Checkings or Savings) and Password strength to be updated.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Customer Feedback for the Frontend Design </t>
   </si>
   <si>
@@ -278,6 +275,25 @@
   </si>
   <si>
     <t>INB 1301</t>
+  </si>
+  <si>
+    <t>Narinder (PM)</t>
+  </si>
+  <si>
+    <t>i. Customer reviewed changes made to the front-end template.</t>
+  </si>
+  <si>
+    <t>i. Narinder &amp; OZ presented the front-end design template to the customer.
+ii. Customer appreciated the team's efforts but pointed out changes to be made, this is shown below</t>
+  </si>
+  <si>
+    <t>i. The user interface lacked consistency in terms of design elements such as color, typography and layout. This can make the application look disjointed and confusing for the user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ii. Some of the design choices may not align with the user's needs and expectations. For example, some of the buttons and menus are not easily discoverable and important information such as account balances are not prominently displayed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">iii. Lastly, I feel the overall design could benefit from more visual hierarchy to guide the user's attention to the most important information and actions. This I believe can be achieved through the use of appropriate sizing, contrast and visual cues. </t>
   </si>
 </sst>
 </file>
@@ -503,7 +519,24 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1129,7 +1162,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B21">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1465,10 +1498,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B12 B14:B22">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="4" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1795,10 +1828,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B12 B16:B21">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="2" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1809,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06FB90B-9967-4372-84C3-A4BAE3D0D22D}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,7 +2045,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="198" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="165" x14ac:dyDescent="0.3">
       <c r="A14" s="41" t="s">
         <v>62</v>
       </c>
@@ -2029,7 +2062,7 @@
         <v>44995</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -2042,7 +2075,7 @@
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="36">
         <v>44998</v>
@@ -2066,7 +2099,7 @@
       <c r="B17" s="5"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" s="36">
         <v>44998</v>
@@ -2084,30 +2117,297 @@
     </row>
     <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="66" x14ac:dyDescent="0.3">
       <c r="A22" s="43" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B14:B18 B11">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="0" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="6" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36106F96-14D2-4754-8A81-8ADE80DA4EDF}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10">
+        <v>44998</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="33">
+        <v>44995</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="36">
+        <v>44998</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="36">
+        <v>44998</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A20" s="43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B11:B16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"open"</formula>
+    </cfRule>
+    <cfRule type="top10" dxfId="0" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2115,21 +2415,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EB80755703E9E4E8871731B0044190C" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6653e26700db3cd95e89e010d55cf40d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5cd8f6c-fbf6-4aca-8ee7-b07d402a0be9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86a0859ca44cdd06f19a56e3da5aad1b" ns2:_="">
     <xsd:import namespace="e5cd8f6c-fbf6-4aca-8ee7-b07d402a0be9"/>
@@ -2273,24 +2558,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46AD8F31-2DCC-457B-A0A0-F35DD21DE423}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC40E77-96DE-4140-BF58-1FB25F9C79C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A618956-9B8D-412A-93B5-5C8C9AF13C93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2306,4 +2589,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC40E77-96DE-4140-BF58-1FB25F9C79C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46AD8F31-2DCC-457B-A0A0-F35DD21DE423}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
meeting note of 13th March Updated with Customer's feedback
</commit_message>
<xml_diff>
--- a/Agile Meetings/minutes.xlsx
+++ b/Agile Meetings/minutes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Pictures\Bank-App\Agile Meetings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14910778-76D6-42ED-89C0-619478B7F342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7005508E-CFEF-4343-9A69-7D5D1F383F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="28Feb23" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -262,15 +262,6 @@
     <t xml:space="preserve">Customer Feedback for the Frontend Design </t>
   </si>
   <si>
-    <t>i. The team did an excellent job in developing the view account detail feature. However I noticed that some of the information displayed may not be necessary for the user, this was pointed out.</t>
-  </si>
-  <si>
-    <t>ii. The team did well with the implementation of the create account functionality. However, I noticed that there were a few bugs that need to be addressed, and we need to make sure that we have thorough testing in place to catch any potential issues.</t>
-  </si>
-  <si>
-    <t>iii. The team did a good job with implementing the transfer from different accounts functionality. However, I noticed that there were some usability issues that need to be addressed, such as the user interface and flow of the transfer process.</t>
-  </si>
-  <si>
     <t>Based on customer feedback, it was suggested that proper review to be done on the frontend design before commencement of Backend</t>
   </si>
   <si>
@@ -278,9 +269,6 @@
   </si>
   <si>
     <t>Narinder (PM)</t>
-  </si>
-  <si>
-    <t>i. Customer reviewed changes made to the front-end template.</t>
   </si>
   <si>
     <t>i. Narinder &amp; OZ presented the front-end design template to the customer.
@@ -294,6 +282,47 @@
   </si>
   <si>
     <t xml:space="preserve">iii. Lastly, I feel the overall design could benefit from more visual hierarchy to guide the user's attention to the most important information and actions. This I believe can be achieved through the use of appropriate sizing, contrast and visual cues. </t>
+  </si>
+  <si>
+    <t>i. Customer reviewed changes made to the front-end template based on previous feedback and provided comments below.</t>
+  </si>
+  <si>
+    <t>Backend Design</t>
+  </si>
+  <si>
+    <t>i. Gideon was placed as the proponent/'Big Boss' to lead the team on this
+ii. He delegated task to team members, explained the tools/framework to be used (Django).
+iii. Team members were assigned a task to do at the backend to ensure everyone participated in the activity.</t>
+  </si>
+  <si>
+    <t>Design of the structural and behavioural diagrams</t>
+  </si>
+  <si>
+    <t>Gideon &amp; Godswill</t>
+  </si>
+  <si>
+    <t>Sonia, Narinder &amp; OZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
+  </si>
+  <si>
+    <t>Godswill &amp; OZ</t>
+  </si>
+  <si>
+    <t>Based on the scope of our project, the following diagrams were suggested for designs: class, sequence, entity-relationship and use-case diagram</t>
+  </si>
+  <si>
+    <t>MVP Release (V 1.0)</t>
+  </si>
+  <si>
+    <t>i. Customer commended the team on the excellent work they have done in incorporating previous feedback on the front-end design of the project. He mentioned that the changes made have greatly improved the user experience, and he appreciated the team's dedication to creating a high quality product.</t>
+  </si>
+  <si>
+    <t>ii. There were few areas where we could further enhance the design. For example, the color scheme could be adjusted to provide better contrast and make important elements stand out more. Additionally, some o the font sizes could be increased to improve readability.</t>
+  </si>
+  <si>
+    <t>iii. Overall, customer was impressed with the team's effort and appreciated the responsiveness to feedback provided. He is confident that the team would create a user-friendly and effective product.</t>
   </si>
 </sst>
 </file>
@@ -405,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -514,6 +543,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1512,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7523102B-4712-4BF0-8A26-A10243FEB37C}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1842,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06FB90B-9967-4372-84C3-A4BAE3D0D22D}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,7 +2094,7 @@
         <v>44995</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -2075,7 +2107,7 @@
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E15" s="36">
         <v>44998</v>
@@ -2099,7 +2131,7 @@
       <c r="B17" s="5"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E17" s="36">
         <v>44998</v>
@@ -2122,17 +2154,17 @@
     </row>
     <row r="22" spans="1:7" ht="66" x14ac:dyDescent="0.3">
       <c r="A22" s="43" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2149,10 +2181,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36106F96-14D2-4754-8A81-8ADE80DA4EDF}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,7 +2193,7 @@
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2217,7 +2249,7 @@
     </row>
     <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>55</v>
@@ -2312,12 +2344,12 @@
       <c r="F11" s="5"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="99" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>26</v>
+      <c r="B12" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>40</v>
@@ -2329,81 +2361,151 @@
         <v>44995</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="66" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:7" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="33">
+        <v>45003</v>
+      </c>
+      <c r="F13" s="45"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="33">
+        <v>45003</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="33">
+        <v>45005</v>
+      </c>
+      <c r="F15" s="45"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="33">
+        <v>45005</v>
+      </c>
+      <c r="F16" s="45"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="36">
-        <v>44998</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="33">
+        <v>45005</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="36">
-        <v>44998</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="33">
+        <v>45005</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="66" x14ac:dyDescent="0.3">
-      <c r="A20" s="43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="43" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
-        <v>73</v>
+    <row r="24" spans="1:7" ht="99" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="A26" s="44" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B11:B16">
+  <conditionalFormatting sqref="B11 B13:B20">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"open"</formula>
     </cfRule>
@@ -2415,6 +2517,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EB80755703E9E4E8871731B0044190C" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6653e26700db3cd95e89e010d55cf40d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5cd8f6c-fbf6-4aca-8ee7-b07d402a0be9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86a0859ca44cdd06f19a56e3da5aad1b" ns2:_="">
     <xsd:import namespace="e5cd8f6c-fbf6-4aca-8ee7-b07d402a0be9"/>
@@ -2558,15 +2669,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2574,6 +2676,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC40E77-96DE-4140-BF58-1FB25F9C79C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A618956-9B8D-412A-93B5-5C8C9AF13C93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2591,14 +2701,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC40E77-96DE-4140-BF58-1FB25F9C79C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46AD8F31-2DCC-457B-A0A0-F35DD21DE423}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
meeting notes of 19th March
</commit_message>
<xml_diff>
--- a/Agile Meetings/minutes.xlsx
+++ b/Agile Meetings/minutes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Pictures\Bank-App\Agile Meetings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7005508E-CFEF-4343-9A69-7D5D1F383F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251B4F86-333A-44F8-BD82-30140C8C99D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="28Feb23" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="04Mar23" sheetId="3" r:id="rId3"/>
     <sheet name="10Mar23" sheetId="4" r:id="rId4"/>
     <sheet name="13Mar23" sheetId="5" r:id="rId5"/>
+    <sheet name="19Mar23" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="95">
   <si>
     <t>Date</t>
   </si>
@@ -323,6 +324,19 @@
   </si>
   <si>
     <t>iii. Overall, customer was impressed with the team's effort and appreciated the responsiveness to feedback provided. He is confident that the team would create a user-friendly and effective product.</t>
+  </si>
+  <si>
+    <t>i. The team reported with update on the system designs and constructive feedback were provided.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narinder </t>
+  </si>
+  <si>
+    <t>Gideon (PM)</t>
+  </si>
+  <si>
+    <t>i. The team reported with their feedback, errors were spotted through pair programming and feedback provided.
+ii. Commit was made to github repository</t>
   </si>
 </sst>
 </file>
@@ -434,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -547,11 +561,31 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1194,7 +1228,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B21">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1530,10 +1564,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B12 B14:B22">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="6" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1860,10 +1894,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B12 B16:B21">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="4" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2169,10 +2203,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B14:B18 B11">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"open"</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="2" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2183,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36106F96-14D2-4754-8A81-8ADE80DA4EDF}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2435,7 +2469,7 @@
       <c r="F16" s="45"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>50</v>
       </c>
@@ -2443,9 +2477,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="37" t="s">
-        <v>71</v>
-      </c>
+      <c r="D17" s="37"/>
       <c r="E17" s="33">
         <v>45005</v>
       </c>
@@ -2506,6 +2538,304 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11 B13:B20">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"open"</formula>
+    </cfRule>
+    <cfRule type="top10" dxfId="2" priority="2" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25DEC5A3-98FE-41ED-ADE3-9DC57705791E}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10">
+        <v>45004</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="33">
+        <v>45003</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="33">
+        <v>45003</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="38"/>
+      <c r="E14" s="33">
+        <v>45005</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="33">
+        <v>45005</v>
+      </c>
+      <c r="F15" s="45"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="33">
+        <v>45005</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="33">
+        <v>45005</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B11 B14:B19">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"open"</formula>
     </cfRule>
@@ -2517,15 +2847,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EB80755703E9E4E8871731B0044190C" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6653e26700db3cd95e89e010d55cf40d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5cd8f6c-fbf6-4aca-8ee7-b07d402a0be9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86a0859ca44cdd06f19a56e3da5aad1b" ns2:_="">
     <xsd:import namespace="e5cd8f6c-fbf6-4aca-8ee7-b07d402a0be9"/>
@@ -2669,6 +2990,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2676,14 +3006,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC40E77-96DE-4140-BF58-1FB25F9C79C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A618956-9B8D-412A-93B5-5C8C9AF13C93}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2701,6 +3023,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC40E77-96DE-4140-BF58-1FB25F9C79C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46AD8F31-2DCC-457B-A0A0-F35DD21DE423}">
   <ds:schemaRefs>

</xml_diff>